<commit_message>
Results and plots for first submission
</commit_message>
<xml_diff>
--- a/input/input_data.xlsx
+++ b/input/input_data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxv/Documents/GitHub/sddp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxv/Documents/GitHub/sddp/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3795BF3C-22B3-F44A-B1DA-6D8F87AF82F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CA8D7C-58C0-AB49-9A22-6504F08C0691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1200" windowWidth="25040" windowHeight="14340" xr2:uid="{9D30D194-77BF-B34D-97C7-0327CCC33E0B}"/>
+    <workbookView xWindow="560" yWindow="1200" windowWidth="25040" windowHeight="14340" xr2:uid="{9D30D194-77BF-B34D-97C7-0327CCC33E0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -463,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA2B3773-D540-714A-BB4D-A08BF0A40297}">
-  <dimension ref="A1:R49"/>
+  <dimension ref="A1:R73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="R74" sqref="R74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,29 +560,29 @@
         <v>0.4</v>
       </c>
       <c r="G2">
-        <f>F2*(1+0.3)</f>
+        <f t="shared" ref="G2:G25" si="1">F2*(1+0.3)</f>
         <v>0.52</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <f xml:space="preserve"> E2 - 0.1</f>
+        <f t="shared" ref="I2:I24" si="2" xml:space="preserve"> E2 - 0.1</f>
         <v>0.17999999999999997</v>
       </c>
       <c r="J2">
-        <f xml:space="preserve"> F2 - 0.1</f>
+        <f t="shared" ref="J2:J24" si="3" xml:space="preserve"> F2 - 0.1</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="K2">
-        <f xml:space="preserve"> G2 - 0.1</f>
+        <f t="shared" ref="K2:K24" si="4" xml:space="preserve"> G2 - 0.1</f>
         <v>0.42000000000000004</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <f xml:space="preserve"> -Q2</f>
+        <f t="shared" ref="M2:M20" si="5" xml:space="preserve"> -Q2</f>
         <v>0</v>
       </c>
       <c r="O2">
@@ -601,15 +601,15 @@
         <v>49.2</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B49" si="1">C3*(1-0.3)</f>
+        <f t="shared" ref="B3:B49" si="6">C3*(1-0.3)</f>
         <v>0.20663999999999999</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C49" si="2" xml:space="preserve"> A3 / 1000 * 6</f>
+        <f t="shared" ref="C3:C49" si="7" xml:space="preserve"> A3 / 1000 * 6</f>
         <v>0.29520000000000002</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D49" si="3">C3*(1+0.3)</f>
+        <f t="shared" ref="D3:D49" si="8">C3*(1+0.3)</f>
         <v>0.38376000000000005</v>
       </c>
       <c r="E3">
@@ -617,33 +617,33 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F4" si="4">0.4</f>
+        <f t="shared" ref="F3:F4" si="9">0.4</f>
         <v>0.4</v>
       </c>
       <c r="G3">
-        <f>F3*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <f xml:space="preserve"> E3 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J3">
-        <f xml:space="preserve"> F3 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K3">
-        <f xml:space="preserve"> G3 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <f xml:space="preserve"> -Q3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O3">
@@ -661,15 +661,15 @@
         <v>44.3</v>
       </c>
       <c r="B4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.18605999999999998</v>
       </c>
       <c r="C4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.26579999999999998</v>
       </c>
       <c r="D4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.34554000000000001</v>
       </c>
       <c r="E4">
@@ -677,33 +677,33 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F4">
+        <f t="shared" si="9"/>
+        <v>0.4</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0.52</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K4">
         <f t="shared" si="4"/>
-        <v>0.4</v>
-      </c>
-      <c r="G4">
-        <f>F4*(1+0.3)</f>
-        <v>0.52</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <f xml:space="preserve"> E4 - 0.1</f>
-        <v>0.17999999999999997</v>
-      </c>
-      <c r="J4">
-        <f xml:space="preserve"> F4 - 0.1</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="K4">
-        <f xml:space="preserve"> G4 - 0.1</f>
         <v>0.42000000000000004</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <f xml:space="preserve"> -Q4</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O4">
@@ -721,15 +721,15 @@
         <v>43.1</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.18101999999999999</v>
       </c>
       <c r="C5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.2586</v>
       </c>
       <c r="D5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.33618000000000003</v>
       </c>
       <c r="E5">
@@ -740,29 +740,29 @@
         <v>0.4</v>
       </c>
       <c r="G5">
-        <f>F5*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <f xml:space="preserve"> E5 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J5">
-        <f xml:space="preserve"> F5 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K5">
-        <f xml:space="preserve"> G5 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <f xml:space="preserve"> -Q5</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O5">
@@ -780,15 +780,15 @@
         <v>44.1</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.18522</v>
       </c>
       <c r="C6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.2646</v>
       </c>
       <c r="D6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.34398000000000001</v>
       </c>
       <c r="E6">
@@ -796,33 +796,33 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F49" si="5">0.4</f>
+        <f t="shared" ref="F6:F49" si="10">0.4</f>
         <v>0.4</v>
       </c>
       <c r="G6">
-        <f>F6*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
-        <f xml:space="preserve"> E6 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J6">
-        <f xml:space="preserve"> F6 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K6">
-        <f xml:space="preserve"> G6 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L6">
         <v>9.8777419354838768E-4</v>
       </c>
       <c r="M6">
-        <f xml:space="preserve"> -Q6</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O6">
@@ -841,15 +841,15 @@
         <v>52.6</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.22091999999999998</v>
       </c>
       <c r="C7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.31559999999999999</v>
       </c>
       <c r="D7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.41027999999999998</v>
       </c>
       <c r="E7">
@@ -860,36 +860,36 @@
         <v>0.5</v>
       </c>
       <c r="G7">
-        <f>F7*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.65</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
-        <f xml:space="preserve"> E7 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="J7">
-        <f xml:space="preserve"> F7 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
       <c r="K7">
-        <f xml:space="preserve"> G7 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="L7">
         <v>2.642175268817205E-2</v>
       </c>
       <c r="M7">
-        <f xml:space="preserve"> -Q7</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="Q7">
-        <f t="shared" ref="Q7:Q20" si="6" xml:space="preserve"> 0.0742 * _xlfn.NORM.DIST( _xlfn.NORM.INV(0.8, 0, 1), 0, 1, FALSE) / (1-(0.8))</f>
+        <f t="shared" ref="Q7:Q20" si="11" xml:space="preserve"> 0.0742 * _xlfn.NORM.DIST( _xlfn.NORM.INV(0.8, 0, 1), 0, 1, FALSE) / (1-(0.8))</f>
         <v>0.10386587247129686</v>
       </c>
       <c r="R7">
@@ -901,15 +901,15 @@
         <v>92.9</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.39018000000000008</v>
       </c>
       <c r="C8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.55740000000000012</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.72462000000000015</v>
       </c>
       <c r="E8">
@@ -917,40 +917,40 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G8">
-        <f>F8*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <f xml:space="preserve"> E8 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J8">
-        <f xml:space="preserve"> F8 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K8">
-        <f xml:space="preserve"> G8 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L8">
         <v>0.1185145698924731</v>
       </c>
       <c r="M8">
-        <f xml:space="preserve"> -Q8</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R8">
@@ -962,15 +962,15 @@
         <v>130</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.54599999999999993</v>
       </c>
       <c r="C9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.78</v>
       </c>
       <c r="D9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.014</v>
       </c>
       <c r="E9">
@@ -981,36 +981,36 @@
         <v>0.2</v>
       </c>
       <c r="G9">
-        <f>F9*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
-        <f xml:space="preserve"> E9 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J9">
-        <f xml:space="preserve"> F9 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="K9">
-        <f xml:space="preserve"> G9 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.16</v>
       </c>
       <c r="L9">
         <v>0.25077729032258073</v>
       </c>
       <c r="M9">
-        <f xml:space="preserve"> -Q9</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R9">
@@ -1022,15 +1022,15 @@
         <v>137</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.57540000000000002</v>
       </c>
       <c r="C10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.82200000000000006</v>
       </c>
       <c r="D10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0686000000000002</v>
       </c>
       <c r="E10">
@@ -1041,36 +1041,36 @@
         <v>0.2</v>
       </c>
       <c r="G10">
-        <f>F10*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
-        <f xml:space="preserve"> E10 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J10">
-        <f xml:space="preserve"> F10 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="K10">
-        <f xml:space="preserve"> G10 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.16</v>
       </c>
       <c r="L10">
         <v>0.37298178494623641</v>
       </c>
       <c r="M10">
-        <f xml:space="preserve"> -Q10</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R10">
@@ -1082,15 +1082,15 @@
         <v>136</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.57120000000000004</v>
       </c>
       <c r="C11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.81600000000000006</v>
       </c>
       <c r="D11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0608000000000002</v>
       </c>
       <c r="E11">
@@ -1101,36 +1101,36 @@
         <v>0.2</v>
       </c>
       <c r="G11">
-        <f>F11*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="I11">
-        <f xml:space="preserve"> E11 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J11">
-        <f xml:space="preserve"> F11 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="K11">
-        <f xml:space="preserve"> G11 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.16</v>
       </c>
       <c r="L11">
         <v>0.46255191397849471</v>
       </c>
       <c r="M11">
-        <f xml:space="preserve"> -Q11</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R11">
@@ -1142,15 +1142,15 @@
         <v>132</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.5544</v>
       </c>
       <c r="C12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.79200000000000004</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0296000000000001</v>
       </c>
       <c r="E12">
@@ -1161,36 +1161,36 @@
         <v>0.2</v>
       </c>
       <c r="G12">
-        <f>F12*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
-        <f xml:space="preserve"> E12 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J12">
-        <f xml:space="preserve"> F12 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="K12">
-        <f xml:space="preserve"> G12 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.16</v>
       </c>
       <c r="L12">
         <v>0.49713122580645169</v>
       </c>
       <c r="M12">
-        <f xml:space="preserve"> -Q12</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R12">
@@ -1202,15 +1202,15 @@
         <v>133</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.55859999999999999</v>
       </c>
       <c r="C13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.79800000000000004</v>
       </c>
       <c r="D13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0374000000000001</v>
       </c>
       <c r="E13">
@@ -1221,36 +1221,36 @@
         <v>0.2</v>
       </c>
       <c r="G13">
-        <f>F13*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13">
-        <f xml:space="preserve"> E13 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J13">
-        <f xml:space="preserve"> F13 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="K13">
-        <f xml:space="preserve"> G13 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.16</v>
       </c>
       <c r="L13">
         <v>0.51404631182795657</v>
       </c>
       <c r="M13">
-        <f xml:space="preserve"> -Q13</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R13">
@@ -1262,15 +1262,15 @@
         <v>150</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.62999999999999989</v>
       </c>
       <c r="C14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="D14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.17</v>
       </c>
       <c r="E14">
@@ -1281,36 +1281,36 @@
         <v>0.2</v>
       </c>
       <c r="G14">
-        <f>F14*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14">
-        <f xml:space="preserve"> E14 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J14">
-        <f xml:space="preserve"> F14 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="K14">
-        <f xml:space="preserve"> G14 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.16</v>
       </c>
       <c r="L14">
         <v>0.50633239784946149</v>
       </c>
       <c r="M14">
-        <f xml:space="preserve"> -Q14</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R14">
@@ -1322,15 +1322,15 @@
         <v>146</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.61319999999999986</v>
       </c>
       <c r="C15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.87599999999999989</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.1387999999999998</v>
       </c>
       <c r="E15">
@@ -1341,36 +1341,36 @@
         <v>0.3</v>
       </c>
       <c r="G15">
-        <f>F15*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.39</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15">
-        <f xml:space="preserve"> E15 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.10999999999999999</v>
       </c>
       <c r="J15">
-        <f xml:space="preserve"> F15 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="K15">
-        <f xml:space="preserve"> G15 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.29000000000000004</v>
       </c>
       <c r="L15">
         <v>0.46419512903225801</v>
       </c>
       <c r="M15">
-        <f xml:space="preserve"> -Q15</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R15">
@@ -1382,15 +1382,15 @@
         <v>127</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.53339999999999999</v>
       </c>
       <c r="C16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.76200000000000001</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.99060000000000004</v>
       </c>
       <c r="E16">
@@ -1398,40 +1398,40 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G16">
-        <f>F16*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16">
-        <f xml:space="preserve"> E16 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J16">
-        <f xml:space="preserve"> F16 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K16">
-        <f xml:space="preserve"> G16 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L16">
         <v>0.389421161290323</v>
       </c>
       <c r="M16">
-        <f xml:space="preserve"> -Q16</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R16">
@@ -1443,15 +1443,15 @@
         <v>113</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.47460000000000002</v>
       </c>
       <c r="C17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.67800000000000005</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.88140000000000007</v>
       </c>
       <c r="E17">
@@ -1459,40 +1459,40 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G17">
-        <f>F17*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17">
-        <f xml:space="preserve"> E17 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J17">
-        <f xml:space="preserve"> F17 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K17">
-        <f xml:space="preserve"> G17 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L17">
         <v>0.30675132258064441</v>
       </c>
       <c r="M17">
-        <f xml:space="preserve"> -Q17</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R17">
@@ -1504,15 +1504,15 @@
         <v>106</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.44519999999999998</v>
       </c>
       <c r="C18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.63600000000000001</v>
       </c>
       <c r="D18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.82680000000000009</v>
       </c>
       <c r="E18">
@@ -1520,40 +1520,40 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G18">
-        <f>F18*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18">
-        <f xml:space="preserve"> E18 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J18">
-        <f xml:space="preserve"> F18 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K18">
-        <f xml:space="preserve"> G18 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L18">
         <v>0.19529535483870969</v>
       </c>
       <c r="M18">
-        <f xml:space="preserve"> -Q18</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R18">
@@ -1565,15 +1565,15 @@
         <v>116</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.48720000000000002</v>
       </c>
       <c r="C19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.69600000000000006</v>
       </c>
       <c r="D19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.90480000000000016</v>
       </c>
       <c r="E19">
@@ -1584,36 +1584,36 @@
         <v>0.6</v>
       </c>
       <c r="G19">
-        <f>F19*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
-        <f xml:space="preserve"> E19 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.31999999999999995</v>
       </c>
       <c r="J19">
-        <f xml:space="preserve"> F19 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K19">
-        <f xml:space="preserve"> G19 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.68</v>
       </c>
       <c r="L19">
         <v>7.8650645161290236E-2</v>
       </c>
       <c r="M19">
-        <f xml:space="preserve"> -Q19</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R19">
@@ -1625,15 +1625,15 @@
         <v>145</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.60899999999999987</v>
       </c>
       <c r="C20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.86999999999999988</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.1309999999999998</v>
       </c>
       <c r="E20">
@@ -1644,36 +1644,36 @@
         <v>0.5</v>
       </c>
       <c r="G20">
-        <f>F20*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.65</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="I20">
-        <f xml:space="preserve"> E20 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="J20">
-        <f xml:space="preserve"> F20 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
       <c r="K20">
-        <f xml:space="preserve"> G20 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="L20">
         <v>1.945845161290323E-2</v>
       </c>
       <c r="M20">
-        <f xml:space="preserve"> -Q20</f>
+        <f t="shared" si="5"/>
         <v>-0.10386587247129686</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.10386587247129686</v>
       </c>
       <c r="R20">
@@ -1685,15 +1685,15 @@
         <v>172</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.72239999999999993</v>
       </c>
       <c r="C21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.032</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.3416000000000001</v>
       </c>
       <c r="E21">
@@ -1704,22 +1704,22 @@
         <v>0.5</v>
       </c>
       <c r="G21">
-        <f>F21*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.65</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
       <c r="I21">
-        <f xml:space="preserve"> E21 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="J21">
-        <f xml:space="preserve"> F21 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
       <c r="K21">
-        <f xml:space="preserve"> G21 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="L21">
@@ -1743,15 +1743,15 @@
         <v>168</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.7056</v>
       </c>
       <c r="C22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.008</v>
       </c>
       <c r="D22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.3104</v>
       </c>
       <c r="E22">
@@ -1762,22 +1762,22 @@
         <v>0.5</v>
       </c>
       <c r="G22">
-        <f>F22*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.65</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22">
-        <f xml:space="preserve"> E22 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="J22">
-        <f xml:space="preserve"> F22 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
       <c r="K22">
-        <f xml:space="preserve"> G22 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="L22">
@@ -1801,15 +1801,15 @@
         <v>156</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.65519999999999989</v>
       </c>
       <c r="C23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.93599999999999994</v>
       </c>
       <c r="D23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.2167999999999999</v>
       </c>
       <c r="E23">
@@ -1817,26 +1817,26 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G23">
-        <f>F23*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
       <c r="I23">
-        <f xml:space="preserve"> E23 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J23">
-        <f xml:space="preserve"> F23 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K23">
-        <f xml:space="preserve"> G23 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L23">
@@ -1860,15 +1860,15 @@
         <v>136</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.57120000000000004</v>
       </c>
       <c r="C24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.81600000000000006</v>
       </c>
       <c r="D24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0608000000000002</v>
       </c>
       <c r="E24">
@@ -1876,26 +1876,26 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G24">
-        <f>F24*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24">
-        <f xml:space="preserve"> E24 - 0.1</f>
+        <f t="shared" si="2"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J24">
-        <f xml:space="preserve"> F24 - 0.1</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K24">
-        <f xml:space="preserve"> G24 - 0.1</f>
+        <f t="shared" si="4"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L24">
@@ -1919,15 +1919,15 @@
         <v>100</v>
       </c>
       <c r="B25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="C25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="D25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.78000000000000014</v>
       </c>
       <c r="E25">
@@ -1935,11 +1935,11 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G25">
-        <f>F25*(1+0.3)</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="H25">
@@ -1954,7 +1954,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:K49" si="7" xml:space="preserve"> G25 - 0.1</f>
+        <f t="shared" ref="K25:K72" si="12" xml:space="preserve"> G25 - 0.1</f>
         <v>0.42000000000000004</v>
       </c>
       <c r="L25">
@@ -1970,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="R25">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1979,15 +1979,15 @@
         <v>66.599999999999994</v>
       </c>
       <c r="B26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.27971999999999997</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.39959999999999996</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.51947999999999994</v>
       </c>
       <c r="E26" s="3">
@@ -1999,22 +1999,22 @@
         <v>0.4</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" ref="G26:G49" si="8">F26*(1+0.3)</f>
+        <f t="shared" ref="G26:G73" si="13">F26*(1+0.3)</f>
         <v>0.52</v>
       </c>
       <c r="H26" s="3">
         <v>1</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" ref="I26:I49" si="9" xml:space="preserve"> E26 - 0.1</f>
+        <f t="shared" ref="I26:I72" si="14" xml:space="preserve"> E26 - 0.1</f>
         <v>0.17999999999999997</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" ref="J26:J49" si="10" xml:space="preserve"> F26 - 0.1</f>
+        <f t="shared" ref="J26:J72" si="15" xml:space="preserve"> F26 - 0.1</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L26" s="3">
@@ -2040,15 +2040,15 @@
         <v>49.2</v>
       </c>
       <c r="B27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.20663999999999999</v>
       </c>
       <c r="C27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.29520000000000002</v>
       </c>
       <c r="D27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.38376000000000005</v>
       </c>
       <c r="E27">
@@ -2056,33 +2056,33 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F27:F28" si="11">0.4</f>
+        <f t="shared" ref="F27:F28" si="16">0.4</f>
         <v>0.4</v>
       </c>
       <c r="G27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27:M44" si="12" xml:space="preserve"> -Q27</f>
+        <f t="shared" ref="M27:M44" si="17" xml:space="preserve"> -Q27</f>
         <v>0</v>
       </c>
       <c r="O27">
@@ -2100,15 +2100,15 @@
         <v>44.3</v>
       </c>
       <c r="B28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.18605999999999998</v>
       </c>
       <c r="C28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.26579999999999998</v>
       </c>
       <c r="D28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.34554000000000001</v>
       </c>
       <c r="E28">
@@ -2116,33 +2116,33 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.4</v>
       </c>
       <c r="G28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O28">
@@ -2160,15 +2160,15 @@
         <v>43.1</v>
       </c>
       <c r="B29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.18101999999999999</v>
       </c>
       <c r="C29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.2586</v>
       </c>
       <c r="D29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.33618000000000003</v>
       </c>
       <c r="E29">
@@ -2179,29 +2179,29 @@
         <v>0.4</v>
       </c>
       <c r="G29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O29">
@@ -2219,15 +2219,15 @@
         <v>44.1</v>
       </c>
       <c r="B30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.18522</v>
       </c>
       <c r="C30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.2646</v>
       </c>
       <c r="D30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.34398000000000001</v>
       </c>
       <c r="E30">
@@ -2235,40 +2235,40 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L30">
         <v>9.8777419354838768E-4</v>
       </c>
       <c r="M30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
       <c r="Q30">
-        <f t="shared" ref="Q30:Q44" si="13" xml:space="preserve"> 0.0742 * _xlfn.NORM.DIST( _xlfn.NORM.INV(2/3, 0, 1), 0, 1, FALSE) / (1-(2/3))</f>
+        <f t="shared" ref="Q30:Q44" si="18" xml:space="preserve"> 0.0742 * _xlfn.NORM.DIST( _xlfn.NORM.INV(2/3, 0, 1), 0, 1, FALSE) / (1-(2/3))</f>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R30">
@@ -2280,15 +2280,15 @@
         <v>52.6</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.22091999999999998</v>
       </c>
       <c r="C31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.31559999999999999</v>
       </c>
       <c r="D31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.41027999999999998</v>
       </c>
       <c r="E31">
@@ -2299,36 +2299,36 @@
         <v>0.5</v>
       </c>
       <c r="G31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.65</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="J31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.4</v>
       </c>
       <c r="K31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="L31">
         <v>2.642175268817205E-2</v>
       </c>
       <c r="M31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R31">
@@ -2340,15 +2340,15 @@
         <v>92.9</v>
       </c>
       <c r="B32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.39018000000000008</v>
       </c>
       <c r="C32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.55740000000000012</v>
       </c>
       <c r="D32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.72462000000000015</v>
       </c>
       <c r="E32">
@@ -2356,40 +2356,40 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L32">
         <v>0.1185145698924731</v>
       </c>
       <c r="M32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O32">
         <v>0</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R32">
@@ -2401,15 +2401,15 @@
         <v>130</v>
       </c>
       <c r="B33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.54599999999999993</v>
       </c>
       <c r="C33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.78</v>
       </c>
       <c r="D33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.014</v>
       </c>
       <c r="E33">
@@ -2420,36 +2420,36 @@
         <v>0.2</v>
       </c>
       <c r="G33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.26</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="K33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.16</v>
       </c>
       <c r="L33">
         <v>0.25077729032258073</v>
       </c>
       <c r="M33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O33">
         <v>0</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R33">
@@ -2461,15 +2461,15 @@
         <v>137</v>
       </c>
       <c r="B34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.57540000000000002</v>
       </c>
       <c r="C34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.82200000000000006</v>
       </c>
       <c r="D34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0686000000000002</v>
       </c>
       <c r="E34">
@@ -2480,36 +2480,36 @@
         <v>0.2</v>
       </c>
       <c r="G34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.26</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="K34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.16</v>
       </c>
       <c r="L34">
         <v>0.37298178494623641</v>
       </c>
       <c r="M34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R34">
@@ -2521,15 +2521,15 @@
         <v>136</v>
       </c>
       <c r="B35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.57120000000000004</v>
       </c>
       <c r="C35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.81600000000000006</v>
       </c>
       <c r="D35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0608000000000002</v>
       </c>
       <c r="E35">
@@ -2540,36 +2540,36 @@
         <v>0.2</v>
       </c>
       <c r="G35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.26</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="K35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.16</v>
       </c>
       <c r="L35">
         <v>0.46255191397849471</v>
       </c>
       <c r="M35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O35">
         <v>0</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R35">
@@ -2581,15 +2581,15 @@
         <v>132</v>
       </c>
       <c r="B36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.5544</v>
       </c>
       <c r="C36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.79200000000000004</v>
       </c>
       <c r="D36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0296000000000001</v>
       </c>
       <c r="E36">
@@ -2600,36 +2600,36 @@
         <v>0.2</v>
       </c>
       <c r="G36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.26</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="K36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.16</v>
       </c>
       <c r="L36">
         <v>0.49713122580645169</v>
       </c>
       <c r="M36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O36">
         <v>0</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R36">
@@ -2641,15 +2641,15 @@
         <v>133</v>
       </c>
       <c r="B37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.55859999999999999</v>
       </c>
       <c r="C37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.79800000000000004</v>
       </c>
       <c r="D37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0374000000000001</v>
       </c>
       <c r="E37">
@@ -2660,36 +2660,36 @@
         <v>0.2</v>
       </c>
       <c r="G37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.26</v>
       </c>
       <c r="H37">
         <v>1</v>
       </c>
       <c r="I37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="K37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.16</v>
       </c>
       <c r="L37">
         <v>0.51404631182795657</v>
       </c>
       <c r="M37">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O37">
         <v>0</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R37">
@@ -2701,15 +2701,15 @@
         <v>150</v>
       </c>
       <c r="B38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.62999999999999989</v>
       </c>
       <c r="C38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="D38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.17</v>
       </c>
       <c r="E38">
@@ -2720,36 +2720,36 @@
         <v>0.2</v>
       </c>
       <c r="G38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.26</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="I38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="J38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.1</v>
       </c>
       <c r="K38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.16</v>
       </c>
       <c r="L38">
         <v>0.50633239784946149</v>
       </c>
       <c r="M38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O38">
         <v>0</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R38">
@@ -2761,15 +2761,15 @@
         <v>146</v>
       </c>
       <c r="B39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.61319999999999986</v>
       </c>
       <c r="C39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.87599999999999989</v>
       </c>
       <c r="D39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.1387999999999998</v>
       </c>
       <c r="E39">
@@ -2780,36 +2780,36 @@
         <v>0.3</v>
       </c>
       <c r="G39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.39</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.10999999999999999</v>
       </c>
       <c r="J39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="K39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.29000000000000004</v>
       </c>
       <c r="L39">
         <v>0.46419512903225801</v>
       </c>
       <c r="M39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O39">
         <v>0</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R39">
@@ -2821,15 +2821,15 @@
         <v>127</v>
       </c>
       <c r="B40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.53339999999999999</v>
       </c>
       <c r="C40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.76200000000000001</v>
       </c>
       <c r="D40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.99060000000000004</v>
       </c>
       <c r="E40">
@@ -2837,40 +2837,40 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L40">
         <v>0.389421161290323</v>
       </c>
       <c r="M40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O40">
         <v>0</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R40">
@@ -2882,15 +2882,15 @@
         <v>113</v>
       </c>
       <c r="B41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.47460000000000002</v>
       </c>
       <c r="C41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.67800000000000005</v>
       </c>
       <c r="D41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.88140000000000007</v>
       </c>
       <c r="E41">
@@ -2898,40 +2898,40 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L41">
         <v>0.30675132258064441</v>
       </c>
       <c r="M41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O41">
         <v>0</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R41">
@@ -2943,15 +2943,15 @@
         <v>106</v>
       </c>
       <c r="B42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.44519999999999998</v>
       </c>
       <c r="C42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.63600000000000001</v>
       </c>
       <c r="D42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.82680000000000009</v>
       </c>
       <c r="E42">
@@ -2959,40 +2959,40 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L42">
         <v>0.19529535483870969</v>
       </c>
       <c r="M42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O42">
         <v>0</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R42">
@@ -3004,15 +3004,15 @@
         <v>116</v>
       </c>
       <c r="B43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.48720000000000002</v>
       </c>
       <c r="C43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.69600000000000006</v>
       </c>
       <c r="D43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.90480000000000016</v>
       </c>
       <c r="E43">
@@ -3023,36 +3023,36 @@
         <v>0.6</v>
       </c>
       <c r="G43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.78</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.31999999999999995</v>
       </c>
       <c r="J43">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.5</v>
       </c>
       <c r="K43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.68</v>
       </c>
       <c r="L43">
         <v>7.8650645161290236E-2</v>
       </c>
       <c r="M43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O43">
         <v>0</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R43">
@@ -3064,15 +3064,15 @@
         <v>145</v>
       </c>
       <c r="B44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.60899999999999987</v>
       </c>
       <c r="C44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.86999999999999988</v>
       </c>
       <c r="D44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.1309999999999998</v>
       </c>
       <c r="E44">
@@ -3083,36 +3083,36 @@
         <v>0.5</v>
       </c>
       <c r="G44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.65</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="J44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.4</v>
       </c>
       <c r="K44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="L44">
         <v>1.945845161290323E-2</v>
       </c>
       <c r="M44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-8.0937309842725721E-2</v>
       </c>
       <c r="O44">
         <v>0</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8.0937309842725721E-2</v>
       </c>
       <c r="R44">
@@ -3124,15 +3124,15 @@
         <v>172</v>
       </c>
       <c r="B45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.72239999999999993</v>
       </c>
       <c r="C45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.032</v>
       </c>
       <c r="D45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.3416000000000001</v>
       </c>
       <c r="E45">
@@ -3143,22 +3143,22 @@
         <v>0.5</v>
       </c>
       <c r="G45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.65</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="J45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.4</v>
       </c>
       <c r="K45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="L45">
@@ -3182,15 +3182,15 @@
         <v>168</v>
       </c>
       <c r="B46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.7056</v>
       </c>
       <c r="C46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1.008</v>
       </c>
       <c r="D46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.3104</v>
       </c>
       <c r="E46">
@@ -3201,22 +3201,22 @@
         <v>0.5</v>
       </c>
       <c r="G46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.65</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="J46">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.4</v>
       </c>
       <c r="K46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="L46">
@@ -3240,15 +3240,15 @@
         <v>156</v>
       </c>
       <c r="B47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.65519999999999989</v>
       </c>
       <c r="C47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.93599999999999994</v>
       </c>
       <c r="D47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.2167999999999999</v>
       </c>
       <c r="E47">
@@ -3256,26 +3256,26 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J47">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L47">
@@ -3299,15 +3299,15 @@
         <v>136</v>
       </c>
       <c r="B48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.57120000000000004</v>
       </c>
       <c r="C48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.81600000000000006</v>
       </c>
       <c r="D48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0608000000000002</v>
       </c>
       <c r="E48">
@@ -3315,26 +3315,26 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L48">
@@ -3358,15 +3358,15 @@
         <v>100</v>
       </c>
       <c r="B49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="C49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="D49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.78000000000000014</v>
       </c>
       <c r="E49">
@@ -3374,26 +3374,26 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="F49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="G49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.52</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.17999999999999997</v>
       </c>
       <c r="J49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000004</v>
       </c>
       <c r="L49">
@@ -3409,7 +3409,1446 @@
         <v>0</v>
       </c>
       <c r="R49">
-        <v>1</v>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <f xml:space="preserve"> 66.6</f>
+        <v>66.599999999999994</v>
+      </c>
+      <c r="B50" s="3">
+        <f>C50*(1-0.3)</f>
+        <v>0.27971999999999997</v>
+      </c>
+      <c r="C50" s="3">
+        <f xml:space="preserve"> A50 / 1000 * 6</f>
+        <v>0.39959999999999996</v>
+      </c>
+      <c r="D50" s="3">
+        <f>C50*(1+0.3)</f>
+        <v>0.51947999999999994</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" ref="E50:E73" si="19">F50*(1-0.3)</f>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F50" s="3">
+        <f>0.4</f>
+        <v>0.4</v>
+      </c>
+      <c r="G50" s="3">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H50" s="3">
+        <v>1</v>
+      </c>
+      <c r="I50" s="3">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J50" s="3">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K50" s="3">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L50" s="3">
+        <v>0</v>
+      </c>
+      <c r="M50" s="3">
+        <f t="shared" ref="M50:M68" si="20" xml:space="preserve"> -Q50</f>
+        <v>0</v>
+      </c>
+      <c r="O50" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="3">
+        <v>0</v>
+      </c>
+      <c r="R50" s="3">
+        <f>0.1</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>49.2</v>
+      </c>
+      <c r="B51">
+        <f t="shared" ref="B51:B73" si="21">C51*(1-0.3)</f>
+        <v>0.20663999999999999</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51:C73" si="22" xml:space="preserve"> A51 / 1000 * 6</f>
+        <v>0.29520000000000002</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ref="D51:D73" si="23">C51*(1+0.3)</f>
+        <v>0.38376000000000005</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F51">
+        <f t="shared" ref="F51:F52" si="24">0.4</f>
+        <v>0.4</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>44.3</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="21"/>
+        <v>0.18605999999999998</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="22"/>
+        <v>0.26579999999999998</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="23"/>
+        <v>0.34554000000000001</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="24"/>
+        <v>0.4</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>43.1</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="21"/>
+        <v>0.18101999999999999</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="22"/>
+        <v>0.2586</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="23"/>
+        <v>0.33618000000000003</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F53">
+        <v>0.4</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>44.1</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="21"/>
+        <v>0.18522</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="22"/>
+        <v>0.2646</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="23"/>
+        <v>0.34398000000000001</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F54">
+        <f t="shared" ref="F54:F73" si="25">0.4</f>
+        <v>0.4</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L54">
+        <v>9.8777419354838768E-4</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <f xml:space="preserve"> 0.0742 * _xlfn.NORM.DIST( _xlfn.NORM.INV(0.8, 0, 1), 0, 1, FALSE) / (1-(0.8))</f>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R54">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>52.6</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="21"/>
+        <v>0.22091999999999998</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="22"/>
+        <v>0.31559999999999999</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="23"/>
+        <v>0.41027999999999998</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="19"/>
+        <v>0.35</v>
+      </c>
+      <c r="F55">
+        <v>0.5</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="13"/>
+        <v>0.65</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="14"/>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="15"/>
+        <v>0.4</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="12"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L55">
+        <v>2.642175268817205E-2</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" ref="Q55:Q68" si="26" xml:space="preserve"> 0.0742 * _xlfn.NORM.DIST( _xlfn.NORM.INV(0.8, 0, 1), 0, 1, FALSE) / (1-(0.8))</f>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R55">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>92.9</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="21"/>
+        <v>0.39018000000000008</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="22"/>
+        <v>0.55740000000000012</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="23"/>
+        <v>0.72462000000000015</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="25"/>
+        <v>0.4</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L56">
+        <v>0.1185145698924731</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R56">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>130</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="21"/>
+        <v>0.54599999999999993</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="22"/>
+        <v>0.78</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="23"/>
+        <v>1.014</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="19"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="F57">
+        <v>0.2</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="13"/>
+        <v>0.26</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="14"/>
+        <v>3.999999999999998E-2</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="12"/>
+        <v>0.16</v>
+      </c>
+      <c r="L57">
+        <v>0.25077729032258073</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R57">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>137</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="21"/>
+        <v>0.57540000000000002</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="22"/>
+        <v>0.82200000000000006</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="23"/>
+        <v>1.0686000000000002</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="19"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="F58">
+        <v>0.2</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="13"/>
+        <v>0.26</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="14"/>
+        <v>3.999999999999998E-2</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="12"/>
+        <v>0.16</v>
+      </c>
+      <c r="L58">
+        <v>0.37298178494623641</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R58">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>136</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="21"/>
+        <v>0.57120000000000004</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="22"/>
+        <v>0.81600000000000006</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="23"/>
+        <v>1.0608000000000002</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="19"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="F59">
+        <v>0.2</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="13"/>
+        <v>0.26</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="14"/>
+        <v>3.999999999999998E-2</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="12"/>
+        <v>0.16</v>
+      </c>
+      <c r="L59">
+        <v>0.46255191397849471</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R59">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>132</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="21"/>
+        <v>0.5544</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="22"/>
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="23"/>
+        <v>1.0296000000000001</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="19"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="F60">
+        <v>0.2</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="13"/>
+        <v>0.26</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="14"/>
+        <v>3.999999999999998E-2</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="12"/>
+        <v>0.16</v>
+      </c>
+      <c r="L60">
+        <v>0.49713122580645169</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R60">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>133</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="21"/>
+        <v>0.55859999999999999</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="22"/>
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="23"/>
+        <v>1.0374000000000001</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="19"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="F61">
+        <v>0.2</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="13"/>
+        <v>0.26</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="14"/>
+        <v>3.999999999999998E-2</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="12"/>
+        <v>0.16</v>
+      </c>
+      <c r="L61">
+        <v>0.51404631182795657</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R61">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>150</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="21"/>
+        <v>0.62999999999999989</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="22"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="23"/>
+        <v>1.17</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="19"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="F62">
+        <v>0.2</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="13"/>
+        <v>0.26</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="14"/>
+        <v>3.999999999999998E-2</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="12"/>
+        <v>0.16</v>
+      </c>
+      <c r="L62">
+        <v>0.50633239784946149</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R62">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>146</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="21"/>
+        <v>0.61319999999999986</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="22"/>
+        <v>0.87599999999999989</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="23"/>
+        <v>1.1387999999999998</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="19"/>
+        <v>0.21</v>
+      </c>
+      <c r="F63">
+        <v>0.3</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="13"/>
+        <v>0.39</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="14"/>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="15"/>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="12"/>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="L63">
+        <v>0.46419512903225801</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R63">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>127</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="21"/>
+        <v>0.53339999999999999</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="22"/>
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="23"/>
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="25"/>
+        <v>0.4</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L64">
+        <v>0.389421161290323</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R64">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>113</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="21"/>
+        <v>0.47460000000000002</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="22"/>
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="23"/>
+        <v>0.88140000000000007</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="25"/>
+        <v>0.4</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L65">
+        <v>0.30675132258064441</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R65">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>106</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="21"/>
+        <v>0.44519999999999998</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="22"/>
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="23"/>
+        <v>0.82680000000000009</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="25"/>
+        <v>0.4</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L66">
+        <v>0.19529535483870969</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R66">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>116</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="21"/>
+        <v>0.48720000000000002</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="22"/>
+        <v>0.69600000000000006</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="23"/>
+        <v>0.90480000000000016</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="19"/>
+        <v>0.42</v>
+      </c>
+      <c r="F67">
+        <v>0.6</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="13"/>
+        <v>0.78</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="14"/>
+        <v>0.31999999999999995</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="15"/>
+        <v>0.5</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="12"/>
+        <v>0.68</v>
+      </c>
+      <c r="L67">
+        <v>7.8650645161290236E-2</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R67">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>145</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="21"/>
+        <v>0.60899999999999987</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="22"/>
+        <v>0.86999999999999988</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="23"/>
+        <v>1.1309999999999998</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="19"/>
+        <v>0.35</v>
+      </c>
+      <c r="F68">
+        <v>0.5</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="13"/>
+        <v>0.65</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="14"/>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="15"/>
+        <v>0.4</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="12"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L68">
+        <v>1.945845161290323E-2</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="20"/>
+        <v>-0.10386587247129686</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="26"/>
+        <v>0.10386587247129686</v>
+      </c>
+      <c r="R68">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>172</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="21"/>
+        <v>0.72239999999999993</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="22"/>
+        <v>1.032</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="23"/>
+        <v>1.3416000000000001</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="19"/>
+        <v>0.35</v>
+      </c>
+      <c r="F69">
+        <v>0.5</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="13"/>
+        <v>0.65</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="14"/>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="15"/>
+        <v>0.4</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="12"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L69">
+        <v>7.0333333333333326E-5</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>168</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="21"/>
+        <v>0.7056</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="22"/>
+        <v>1.008</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="23"/>
+        <v>1.3104</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="19"/>
+        <v>0.35</v>
+      </c>
+      <c r="F70">
+        <v>0.5</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="13"/>
+        <v>0.65</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="14"/>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="15"/>
+        <v>0.4</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="12"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <v>0</v>
+      </c>
+      <c r="R70">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>156</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="21"/>
+        <v>0.65519999999999989</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="22"/>
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="23"/>
+        <v>1.2167999999999999</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="25"/>
+        <v>0.4</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>136</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="21"/>
+        <v>0.57120000000000004</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="22"/>
+        <v>0.81600000000000006</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="23"/>
+        <v>1.0608000000000002</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="25"/>
+        <v>0.4</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="14"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="12"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
+        <v>0</v>
+      </c>
+      <c r="R72">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>100</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="21"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="22"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="23"/>
+        <v>0.78000000000000014</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="19"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="25"/>
+        <v>0.4</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <f xml:space="preserve"> E73 - 0.1</f>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="J73">
+        <f xml:space="preserve"> F73 - 0.1</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K73">
+        <f t="shared" ref="K73" si="27" xml:space="preserve"> G73 - 0.1</f>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>0</v>
+      </c>
+      <c r="Q73">
+        <v>0</v>
+      </c>
+      <c r="R73">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>